<commit_message>
Adicionada Informações do Dia 27/04/2017
Pesquisas sobre scripts no Unity 3D
</commit_message>
<xml_diff>
--- a/Relatório de Estágio.xlsx
+++ b/Relatório de Estágio.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Abril" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Maio" sheetId="5" r:id="rId2"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Data</t>
   </si>
@@ -79,6 +80,12 @@
   </si>
   <si>
     <t>Trabalhando com scripts para controlar objetos</t>
+  </si>
+  <si>
+    <t>Relatório de Estágio (Maio)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -88,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -136,11 +151,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,10 +219,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,7 +539,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -531,7 +595,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" ref="D6:D19" si="0">C6-B6</f>
+        <f t="shared" ref="D6:D16" si="0">C6-B6</f>
         <v>0.16666666666666669</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -730,83 +794,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" s="2">
         <v>42852</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7">
+      <c r="B16" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D16" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="8">
-        <f>SUM(D5:D19)</f>
-        <v>1.3541666666666667</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickBot="1">
+      <c r="C17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11">
+        <f>SUM(D5:D16)</f>
+        <v>1.4375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -816,13 +853,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="83.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickBot="1">
+      <c r="C17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="11">
+        <f>SUM(D5:D16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -836,4 +1035,16 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>